<commit_message>
add: upload solution function
</commit_message>
<xml_diff>
--- a/Documents/Task.xlsx
+++ b/Documents/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CEBB2E8-4A37-FB43-8C0F-B61F0DAA4916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC660536-213B-6942-9FB0-C4CBD1028502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FB1E2334-D60B-1944-804B-BF7A6A1178BC}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,6 +535,8 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
@@ -543,6 +545,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
@@ -551,6 +555,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -562,6 +568,11 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" t="s">

</xml_diff>